<commit_message>
Update excel templates of input parameters
</commit_message>
<xml_diff>
--- a/inst/xlsx/macrounchainedFocusGW-documentation.xlsx
+++ b/inst/xlsx/macrounchainedFocusGW-documentation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -70,6 +70,21 @@
     <t xml:space="preserve">Columns in ‘s’</t>
   </si>
   <si>
+    <t xml:space="preserve">soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the FOCUS-scenario (soil/ site) to be used for the parameter set. Can only be used when the argument "focus_mode" is set "gw". When the column “soil” is provided, the column "crop" should be provided too (see below), but the argument "parfile" should not be used, and neither the optional column "parfile", as the template par-file is determined internally. Partial matching and transliteration are used, and casing is ignored, and so that input like "Châteaudun", "chateaudun" or "chat" will all refer to the same  Châteaudun FOCUS-scenario. An error will be raised in case of multiple matches or no match.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the FOCUS-crop to be used for the parameter set. Can only be used when the argument "focus_mode" is set to "gw". When the column “crop” is provided, the column "soil" should be provided too (see above). Partial matching and transliteration are used, and casing is ignored. Important qualifiers such as "winter" and "spring" (for cereals and oil seed rape), or "bulb", "fruiting", "leafy" and "root" (for vegetables), should be separated from the crop name by a comma (as in MACRO In FOCUS user interface), but the can come either before or after the crop name. Spaces are otherwise ignored. Input like "Cereals, Winter", "cereals, winter", "cer, win" or even "win, cer" will all refer to the same Winter cereals FOCUS-crop. "Sugar beets" is equivalent to "sugarbeets". An error will be raised in case of multiple matches or no match.</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -77,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">Unique identifier of the substance. Integer between 1 and 998. Will also be used as a Run ID.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">Name of the substance. Names don’t need to be unique, but it may be a good idea if they are.</t>
@@ -409,17 +421,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.05"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -498,7 +510,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="115" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -513,20 +525,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="149.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>21</v>
@@ -534,203 +546,229 @@
       <c r="C9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="C22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="C23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>59</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>